<commit_message>
changes to analysis scripts
- corrected some variable calculations in analysis script

- incorporated automatic downloading of data from the google drive directory

- added rendering of full data to csv

- raw experiment 2 data directory update
</commit_message>
<xml_diff>
--- a/data/experiment-2-raw-data/Statistics-trial-0.xlsx
+++ b/data/experiment-2-raw-data/Statistics-trial-0.xlsx
@@ -424,70 +424,75 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
+          <t>Independent Variable</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>Distance moved</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Velocity</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>periphery</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>periphery</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>periphery</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>center</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>center</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>center</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>left object</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>left object</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>left object</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>right object</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>right object</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>right object</t>
         </is>
@@ -526,70 +531,75 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Independent Variable</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>center-point</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>center-point</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Any of S 1, S 2, S 3, S 4, S 5, S 6, S 7, S 8, S 9, S 16, S 17, S 24, S 25, S 26, S 27, S 28, S 29, S 30, S 31, S 32 / center-point</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Any of S 1, S 2, S 3, S 4, S 5, S 6, S 7, S 8, S 9, S 16, S 17, S 24, S 25, S 26, S 27, S 28, S 29, S 30, S 31, S 32 / center-point</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Any of S 1, S 2, S 3, S 4, S 5, S 6, S 7, S 8, S 9, S 16, S 17, S 24, S 25, S 26, S 27, S 28, S 29, S 30, S 31, S 32 / center-point</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Any of S 10, S 11, S 12, S 13, S 14, S 15, S 18, S 19, S 20, S 21, S 22, S 23 / center-point</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>Any of S 10, S 11, S 12, S 13, S 14, S 15, S 18, S 19, S 20, S 21, S 22, S 23 / center-point</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Any of S 10, S 11, S 12, S 13, S 14, S 15, S 18, S 19, S 20, S 21, S 22, S 23 / center-point</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>left object / center-point</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>left object / center-point</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>left object / center-point</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>right object / center-point</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>right object / center-point</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>right object / center-point</t>
         </is>
@@ -618,80 +628,85 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>object.pair</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>object.side</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>trial</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Cumulative Duration</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Latency to First</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>Cumulative Duration</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>Latency to First</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Cumulative Duration</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>Latency to First</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>Frequency</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>Cumulative Duration</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>Latency to First</t>
         </is>
@@ -730,70 +745,75 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t/>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>cm</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>cm/s</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>s</t>
         </is>
@@ -822,54 +842,59 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>803.308</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2.67686</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>21</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>145.743</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>11.0108</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>21</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>154.551</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>0</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>9</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>47.2463</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>32.4318</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>7</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>22.2218</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>19.6192</v>
       </c>
     </row>
@@ -896,54 +921,59 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1335.94</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>4.45176</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>9</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>288.082</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>8</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>12.212</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>8.80862</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>13</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>42.2414</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>8.00784</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>9</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>19.0186</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>30.2296</v>
       </c>
     </row>
@@ -970,54 +1000,59 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1053.92</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>3.51197</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>15</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>230.426</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>3.20314</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>15</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>69.8684</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>0</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>10</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>34.0333</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>13.8135</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>9</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>30.2296</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>42.8419</v>
       </c>
     </row>
@@ -1044,54 +1079,59 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1408.19</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>4.71451</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>8</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>283.478</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>7</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>16.0157</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>23.6231</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>9</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>18.418</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>15.6153</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>10</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>22.422</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>0</v>
       </c>
     </row>
@@ -1118,54 +1158,59 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1300.57</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>4.33387</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>10</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>273.468</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>9</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>26.8263</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>11.211</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>11</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>27.0265</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>24.8243</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>12</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>40.84</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>0</v>
       </c>
     </row>
@@ -1192,54 +1237,59 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1139.34</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>3.79663</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>13</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>254.049</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>12</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>46.2453</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>15.0147</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>17</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>47.0461</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>34.4337</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>11</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>31.8312</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>4.40431</v>
       </c>
     </row>
@@ -1266,54 +1316,59 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>906.284</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>3.02202</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>14</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>225.421</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>0</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>13</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>74.8733</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>4.40431</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>8</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>22.6221</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>0</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>10</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>52.4514</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>49.8488</v>
       </c>
     </row>
@@ -1340,54 +1395,59 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1271.1</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>4.24416</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>15</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>248.844</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>2.80274</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>15</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>51.4504</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>0</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>10</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <v>32.0314</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>30.63</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>7</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>27.8272</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>0</v>
       </c>
     </row>
@@ -1414,54 +1474,59 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>1505.29</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>5.01606</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>9</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>255.25</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>0</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>8</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>45.0441</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>12.212</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>16</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>44.0431</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>17.2169</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>11</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>26.6261</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>48.6476</v>
       </c>
     </row>
@@ -1488,54 +1553,59 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>1802.95</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>6.00795</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>9</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>279.273</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>8</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>21.0206</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>20.6202</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>14</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>32.6319</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>15.6153</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>14</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>27.0265</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>3.40333</v>
       </c>
     </row>
@@ -1562,54 +1632,59 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>1713.14</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>5.7087</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>6</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>287.882</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>5</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>12.4122</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>0.600588</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>14</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>26.4259</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>0</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>14</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>34.2335</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>5.80568</v>
       </c>
     </row>
@@ -1636,54 +1711,59 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1373.95</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>4.57839</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>9</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>283.678</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>0</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>8</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>16.6163</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>1.20118</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>12</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>25.4249</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>1.80176</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>6</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>23.8233</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>11.6114</v>
       </c>
     </row>
@@ -1710,54 +1790,59 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>left</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>948.2</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>3.15968</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>16</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>252.848</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>0</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>15</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>47.4465</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>0.200196</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>11</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>47.8468</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>0</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>10</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>33.2325</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>15.4151</v>
       </c>
     </row>
@@ -1784,54 +1869,59 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>1189.17</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>3.96267</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>9</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>253.849</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>15.6153</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>9</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>46.4455</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>0</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>9</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>28.2276</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>59.8586</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>8</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>30.0294</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <v>28.628</v>
       </c>
     </row>
@@ -1858,54 +1948,59 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>1482.07</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>4.93868</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>6</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>290.084</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>0</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>5</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>10.21</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>21.8214</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <v>15</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>31.0304</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>2.20216</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>10</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>24.0235</v>
       </c>
-      <c r="T19">
+      <c r="U19">
         <v>9.8096</v>
       </c>
     </row>
@@ -1932,54 +2027,59 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>pair-a</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>right</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>1488.68</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>4.9607</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>8</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>278.873</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>2.00196</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>8</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>21.421</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>0</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>16</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>41.2404</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>4.8047</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>10</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>25.4249</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <v>15.6153</v>
       </c>
     </row>

</xml_diff>